<commit_message>
feat: question crud ops
</commit_message>
<xml_diff>
--- a/public/output/devops-automation.xlsx
+++ b/public/output/devops-automation.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,139 +410,67 @@
         <v>Title</v>
       </c>
       <c r="C1" t="str">
-        <v>Correct</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Choice_1</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Choice_2</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Choice_3</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Choice_4</v>
+        <v>Answer</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>MCQ</v>
+        <v>OpenQuestion</v>
       </c>
       <c r="B2" t="str">
-        <v>What is the first step in the Git Workflow as described in the DevOps Automation lecture notes?</v>
+        <v>What is the first step in the Git Workflow described in the devops automation lecture notes?</v>
       </c>
       <c r="C2" t="str">
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <v/>
-      </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v/>
+        <v>Clone code from the project’s shared repository hosted on a server, e.g., GitHub .</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>MCQ</v>
+        <v>OpenQuestion</v>
       </c>
       <c r="B3" t="str">
-        <v>In the Git Workflow, what is typically done after running unit testing locally?</v>
+        <v>In the Git Workflow example provided, what is the purpose of creating multiple branches for different users working on the project?</v>
       </c>
       <c r="C3" t="str">
-        <v/>
-      </c>
-      <c r="D3" t="str">
-        <v/>
-      </c>
-      <c r="E3" t="str">
-        <v/>
-      </c>
-      <c r="F3" t="str">
-        <v/>
-      </c>
-      <c r="G3" t="str">
-        <v/>
+        <v>Each user can work on their own branch to experiment with new features without affecting others and to maintain flexibility in collaboration .</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>MCQ</v>
+        <v>OpenQuestion</v>
       </c>
       <c r="B4" t="str">
-        <v>According to the lecture notes, what is the purpose of creating a branch for a new user story in Git branching and merging?</v>
+        <v>How is a critical issue handled in the Git Workflow example when working on a project?</v>
       </c>
       <c r="C4" t="str">
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <v/>
-      </c>
-      <c r="E4" t="str">
-        <v/>
-      </c>
-      <c r="F4" t="str">
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <v/>
+        <v>Switch to the production branch, create a new branch to add the fix, test the fix, merge the fix branch, and push to production .</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>MCQ</v>
+        <v>OpenQuestion</v>
       </c>
       <c r="B5" t="str">
-        <v>What is the next step after fixing an urgent production issue in Git branching and merging, based on the notes?</v>
+        <v>What is the purpose of a three-way merge in Git, as described in the lecture notes?</v>
       </c>
       <c r="C5" t="str">
-        <v/>
-      </c>
-      <c r="D5" t="str">
-        <v/>
-      </c>
-      <c r="E5" t="str">
-        <v/>
-      </c>
-      <c r="F5" t="str">
-        <v/>
-      </c>
-      <c r="G5" t="str">
-        <v/>
+        <v>A three-way merge is used to merge branches where a common ancestor is considered along with the two branches to be merged, creating a new commit from the merge .</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>MCQ</v>
+        <v>OpenQuestion</v>
       </c>
       <c r="B6" t="str">
-        <v>In Continuous Integration implementation, what should be done when the build is broken?</v>
+        <v>What is the significance of Continuous Integration (CI) implementation in the Git Workflow process?</v>
       </c>
       <c r="C6" t="str">
-        <v/>
-      </c>
-      <c r="D6" t="str">
-        <v/>
-      </c>
-      <c r="E6" t="str">
-        <v/>
-      </c>
-      <c r="F6" t="str">
-        <v/>
-      </c>
-      <c r="G6" t="str">
-        <v/>
+        <v>CI implementation involves monitoring and reacting to new commits, triggering the build/test process automatically on every push to the main repository, and ensuring integration of changes daily .</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>